<commit_message>
Se agrega documentacion y lotes de pruebas
</commit_message>
<xml_diff>
--- a/Documentacion/Analisis de rendimiento.xlsx
+++ b/Documentacion/Analisis de rendimiento.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolás\Desktop\Programacion Avanzada\TPS\Matriz-VectorMath\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultad\Programacion Avanzada\Matriz-VectorMath\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,10 +317,10 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>447</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3642</c:v>
+                  <c:v>3396</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>23502</c:v>
@@ -343,11 +343,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="162846064"/>
-        <c:axId val="162846456"/>
+        <c:axId val="206810768"/>
+        <c:axId val="206811328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="162846064"/>
+        <c:axId val="206810768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -453,12 +453,12 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162846456"/>
+        <c:crossAx val="206811328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="162846456"/>
+        <c:axId val="206811328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -568,7 +568,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="162846064"/>
+        <c:crossAx val="206810768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1218,7 +1218,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C74A11AD-B747-4EA5-960D-9F6D0927FA16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C74A11AD-B747-4EA5-960D-9F6D0927FA16}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1538,18 +1538,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>10</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>50</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>100</v>
       </c>
@@ -1608,31 +1608,31 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>500</v>
       </c>
       <c r="B6" s="1">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>0.44700000000000001</v>
+        <v>0.435</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1000</v>
       </c>
       <c r="B7" s="1">
-        <v>3642</v>
+        <v>3396</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>3.6419999999999999</v>
+        <v>3.3959999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>2000</v>
       </c>

</xml_diff>